<commit_message>
adding reactors and civilian dock
</commit_message>
<xml_diff>
--- a/parts/src/main/resources/PARTS.xlsx
+++ b/parts/src/main/resources/PARTS.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1880" windowWidth="49640" windowHeight="25040" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1560" yWindow="1880" windowWidth="49640" windowHeight="25040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="PART" sheetId="1" r:id="rId1"/>
     <sheet name="MODEL" sheetId="2" r:id="rId2"/>
-    <sheet name="RESOURCE" sheetId="5" r:id="rId3"/>
+    <sheet name="INTERNAL" sheetId="8" r:id="rId3"/>
+    <sheet name="RESOURCE" sheetId="5" r:id="rId4"/>
+    <sheet name="MODULE" sheetId="6" r:id="rId5"/>
+    <sheet name="CONVERSION" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="204">
   <si>
     <t>name</t>
   </si>
@@ -498,12 +501,198 @@
   <si>
     <t>wasteWaterContainer , CivilianPopulation/Models/Utility/biomassTank</t>
   </si>
+  <si>
+    <t>CivPopReactor</t>
+  </si>
+  <si>
+    <t>EnrichedUranium</t>
+  </si>
+  <si>
+    <t>DepletedUranium</t>
+  </si>
+  <si>
+    <t>XenonGas</t>
+  </si>
+  <si>
+    <t>isTweakable</t>
+  </si>
+  <si>
+    <t>rabidninjawombat</t>
+  </si>
+  <si>
+    <t>0.0, 3.35, 0.0, 0.0, 1.0, 0.0, 2</t>
+  </si>
+  <si>
+    <t>0.0, -3.35, 0.0, 0.0, -1.0, 0.0, 2</t>
+  </si>
+  <si>
+    <t>Netherdyne Reactor Unit DX-110</t>
+  </si>
+  <si>
+    <t>Netherdye</t>
+  </si>
+  <si>
+    <t>The DX-110 is a massive reactor that should provide all the power needed for a interplanetary generation ship.</t>
+  </si>
+  <si>
+    <t>1,1,1,0,0</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>ModuleResourceConverter</t>
+  </si>
+  <si>
+    <t>ConverterName</t>
+  </si>
+  <si>
+    <t>Reactor</t>
+  </si>
+  <si>
+    <t>StartActionName</t>
+  </si>
+  <si>
+    <t>Start Reactor</t>
+  </si>
+  <si>
+    <t>StopActionName</t>
+  </si>
+  <si>
+    <t>Stop Reactor</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>INPUT</t>
+  </si>
+  <si>
+    <t>ResourceName</t>
+  </si>
+  <si>
+    <t>0.0000125</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>OUTPUT</t>
+  </si>
+  <si>
+    <t>0.0000085</t>
+  </si>
+  <si>
+    <t>DumpExcess</t>
+  </si>
+  <si>
+    <t>0.000050</t>
+  </si>
+  <si>
+    <t>ModuleAnimationGroup</t>
+  </si>
+  <si>
+    <t>activeAnimationName</t>
+  </si>
+  <si>
+    <t>reactorOnline</t>
+  </si>
+  <si>
+    <t>Converter</t>
+  </si>
+  <si>
+    <t>autoDeploy</t>
+  </si>
+  <si>
+    <t>deployAnimationName</t>
+  </si>
+  <si>
+    <t>moduleType</t>
+  </si>
+  <si>
+    <t>SmallCivPopReactor</t>
+  </si>
+  <si>
+    <t>0.0, -2.2, 0.0, 0.0, -1.0, 0.0, 1</t>
+  </si>
+  <si>
+    <t>0.0, 2.55, 0.0, 0.0, 1.0, 0.0, 1</t>
+  </si>
+  <si>
+    <t>Netherdyne Reactor Unit MX-99</t>
+  </si>
+  <si>
+    <t>The MX-99 is a smaller version of the its bigger brother the DX-110.  Ment for smaller Civilian ships. </t>
+  </si>
+  <si>
+    <t>reactorOnlineSml</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Electrical/reactor</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Electrical/SmallReactor</t>
+  </si>
+  <si>
+    <t>civieDock</t>
+  </si>
+  <si>
+    <t>0.0, 1, 0.0, 0.0, 1.0, 0.0, 2</t>
+  </si>
+  <si>
+    <t>0.0, -1, 0.0, 0.0, -1.0, 0.0, 2</t>
+  </si>
+  <si>
+    <t>0.0, -1, 0, 0.0, -1, 0, 2</t>
+  </si>
+  <si>
+    <t>Civilian Contractor Dock Mk1</t>
+  </si>
+  <si>
+    <t>Nagoya-Goliath Kolonization Division</t>
+  </si>
+  <si>
+    <t>For stations in orbit around Kerbin and her moons it is feasible to sub-contract civilian transport to facilities.  This module allows new civilians to arrive on the base.</t>
+  </si>
+  <si>
+    <t>CivilianDockGrowth</t>
+  </si>
+  <si>
+    <t>populationGrowthModifier</t>
+  </si>
+  <si>
+    <t>0.000000545</t>
+  </si>
+  <si>
+    <t>KerbalRecruitment</t>
+  </si>
+  <si>
+    <t>CivilianGrowthCounter</t>
+  </si>
+  <si>
+    <t>crewCabinInternals</t>
+  </si>
+  <si>
+    <t>vesselType</t>
+  </si>
+  <si>
+    <t>Ship</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Utility/civiedock</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -538,6 +727,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF2600"/>
+      <name val="Monaco"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -563,7 +757,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -571,6 +765,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -854,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE54"/>
+  <dimension ref="A1:AG82"/>
   <sheetViews>
-    <sheetView zoomScale="84" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -867,36 +1062,38 @@
     <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="34" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="163.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="34" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="163.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -913,85 +1110,91 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1007,71 +1210,71 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="1">
+      <c r="R2" s="1">
         <v>10400</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="S2" s="1">
         <v>180000</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U2" s="1">
+      <c r="W2" s="1">
         <v>7</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="AA2" s="1">
         <v>2</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="AB2" s="1">
         <v>24</v>
       </c>
-      <c r="AA2" s="1">
+      <c r="AC2" s="1">
         <v>2000</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AD2" s="1">
         <v>2000</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AE2" s="1">
         <v>2900</v>
       </c>
-      <c r="AD2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -1087,71 +1290,71 @@
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="1">
+      <c r="R3" s="1">
         <v>10400</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="S3" s="1">
         <v>180000</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U3" s="1">
+      <c r="W3" s="1">
         <v>12</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="AA3" s="1">
         <v>2</v>
       </c>
-      <c r="Z3" s="1">
+      <c r="AB3" s="1">
         <v>24</v>
       </c>
-      <c r="AA3" s="1">
+      <c r="AC3" s="1">
         <v>2000</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AD3" s="1">
         <v>2000</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AE3" s="1">
         <v>2900</v>
       </c>
-      <c r="AD3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AF3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -1167,65 +1370,65 @@
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="1">
+      <c r="R4" s="1">
         <v>10400</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="S4" s="1">
         <v>180000</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U4" s="1">
+      <c r="W4" s="1">
         <v>8</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="AA4" s="1">
         <v>2</v>
       </c>
-      <c r="Z4" s="1">
+      <c r="AB4" s="1">
         <v>24</v>
       </c>
-      <c r="AA4" s="1">
+      <c r="AC4" s="1">
         <v>2000</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AD4" s="1">
         <v>2000</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AE4" s="1">
         <v>2900</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AG4" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>57</v>
       </c>
@@ -1241,71 +1444,71 @@
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="1">
+      <c r="R5" s="1">
         <v>10400</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="S5" s="1">
         <v>180000</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U5" s="1">
+      <c r="W5" s="1">
         <v>4</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="Y5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="Z5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y5" s="1">
+      <c r="AA5" s="1">
         <v>2</v>
       </c>
-      <c r="Z5" s="1">
+      <c r="AB5" s="1">
         <v>32</v>
       </c>
-      <c r="AA5" s="1">
+      <c r="AC5" s="1">
         <v>2000</v>
       </c>
-      <c r="AB5" s="1">
+      <c r="AD5" s="1">
         <v>2000</v>
       </c>
-      <c r="AC5" s="1">
+      <c r="AE5" s="1">
         <v>2900</v>
       </c>
-      <c r="AD5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AF5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>62</v>
       </c>
@@ -1321,71 +1524,71 @@
       <c r="E6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="N6" s="1">
-        <v>0</v>
-      </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="1">
+      <c r="R6" s="1">
         <v>10400</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="S6" s="1">
         <v>180000</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="U6" s="1">
+      <c r="W6" s="1">
         <v>3</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="Z6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="AA6" s="1">
         <v>2</v>
       </c>
-      <c r="Z6" s="1">
+      <c r="AB6" s="1">
         <v>24</v>
       </c>
-      <c r="AA6" s="1">
+      <c r="AC6" s="1">
         <v>20000</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AD6" s="1">
         <v>20000</v>
       </c>
-      <c r="AC6" s="1">
+      <c r="AE6" s="1">
         <v>2900</v>
       </c>
-      <c r="AD6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="1" t="s">
+      <c r="AF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>69</v>
       </c>
@@ -1401,71 +1604,71 @@
       <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P7" s="1">
+      <c r="R7" s="1">
         <v>10400</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="S7" s="1">
         <v>180000</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U7" s="1">
+      <c r="W7" s="1">
         <v>7</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="Y7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="Z7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y7" s="1">
+      <c r="AA7" s="1">
         <v>2</v>
       </c>
-      <c r="Z7" s="1">
+      <c r="AB7" s="1">
         <v>20</v>
       </c>
-      <c r="AA7" s="1">
+      <c r="AC7" s="1">
         <v>2000</v>
       </c>
-      <c r="AB7" s="1">
+      <c r="AD7" s="1">
         <v>2000</v>
       </c>
-      <c r="AC7" s="1">
+      <c r="AE7" s="1">
         <v>2900</v>
       </c>
-      <c r="AD7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>73</v>
       </c>
@@ -1481,71 +1684,71 @@
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N8" s="1">
-        <v>0</v>
-      </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P8" s="1">
+      <c r="R8" s="1">
         <v>10400</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="S8" s="1">
         <v>180000</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="V8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U8" s="1">
+      <c r="W8" s="1">
         <v>7</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="X8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="Y8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="Z8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y8" s="1">
+      <c r="AA8" s="1">
         <v>2</v>
       </c>
-      <c r="Z8" s="1">
+      <c r="AB8" s="1">
         <v>20</v>
       </c>
-      <c r="AA8" s="1">
+      <c r="AC8" s="1">
         <v>2000</v>
       </c>
-      <c r="AB8" s="1">
+      <c r="AD8" s="1">
         <v>2000</v>
       </c>
-      <c r="AC8" s="1">
+      <c r="AE8" s="1">
         <v>2900</v>
       </c>
-      <c r="AD8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="1" t="s">
+      <c r="AF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>76</v>
       </c>
@@ -1561,71 +1764,71 @@
       <c r="E9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="N9" s="1">
-        <v>0</v>
-      </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P9" s="1">
+      <c r="R9" s="1">
         <v>10400</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="S9" s="1">
         <v>180000</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U9" s="1">
+      <c r="W9" s="1">
         <v>7</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="X9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="Y9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X9" s="1" t="s">
+      <c r="Z9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y9" s="1">
+      <c r="AA9" s="1">
         <v>2</v>
       </c>
-      <c r="Z9" s="1">
+      <c r="AB9" s="1">
         <v>20</v>
       </c>
-      <c r="AA9" s="1">
+      <c r="AC9" s="1">
         <v>2000</v>
       </c>
-      <c r="AB9" s="1">
+      <c r="AD9" s="1">
         <v>2000</v>
       </c>
-      <c r="AC9" s="1">
+      <c r="AE9" s="1">
         <v>2900</v>
       </c>
-      <c r="AD9" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="1" t="s">
+      <c r="AF9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>92</v>
       </c>
@@ -1641,83 +1844,83 @@
       <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="N10" s="1">
-        <v>0</v>
-      </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="P10" s="1">
+      <c r="R10" s="1">
         <v>10400</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="S10" s="1">
         <v>22000</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="Y10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X10" s="1" t="s">
+      <c r="Z10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y10" s="1">
+      <c r="AA10" s="1">
         <v>2</v>
       </c>
-      <c r="Z10" s="1">
+      <c r="AB10" s="1">
         <v>30</v>
       </c>
-      <c r="AA10" s="1">
+      <c r="AC10" s="1">
         <v>600</v>
       </c>
-      <c r="AB10" s="1">
+      <c r="AD10" s="1">
         <v>600</v>
       </c>
-      <c r="AC10" s="1">
+      <c r="AE10" s="1">
         <v>2900</v>
       </c>
-      <c r="AE10" s="1" t="s">
+      <c r="AG10" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>113</v>
       </c>
@@ -1733,71 +1936,71 @@
       <c r="E11" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="N11" s="1">
-        <v>0</v>
-      </c>
-      <c r="O11" s="1" t="s">
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P11" s="1">
+      <c r="R11" s="1">
         <v>10400</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="S11" s="1">
         <v>180000</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="T11" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="U11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="V11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U11" s="1">
+      <c r="W11" s="1">
         <v>4</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="X11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="Y11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X11" s="1" t="s">
+      <c r="Z11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y11" s="1">
+      <c r="AA11" s="1">
         <v>2</v>
       </c>
-      <c r="Z11" s="1">
+      <c r="AB11" s="1">
         <v>18</v>
       </c>
-      <c r="AA11" s="1">
+      <c r="AC11" s="1">
         <v>2000</v>
       </c>
-      <c r="AB11" s="1">
+      <c r="AD11" s="1">
         <v>2000</v>
       </c>
-      <c r="AC11" s="1">
+      <c r="AE11" s="1">
         <v>2900</v>
       </c>
-      <c r="AD11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="1" t="s">
+      <c r="AF11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>119</v>
       </c>
@@ -1813,71 +2016,71 @@
       <c r="E12" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="N12" s="1">
-        <v>0</v>
-      </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P12" s="1">
+      <c r="R12" s="1">
         <v>10400</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="S12" s="1">
         <v>320000</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="U12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="V12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U12" s="1">
+      <c r="W12" s="1">
         <v>8</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="X12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W12" s="1" t="s">
+      <c r="Y12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X12" s="1" t="s">
+      <c r="Z12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y12" s="1">
+      <c r="AA12" s="1">
         <v>2</v>
       </c>
-      <c r="Z12" s="1">
+      <c r="AB12" s="1">
         <v>20</v>
       </c>
-      <c r="AA12" s="1">
+      <c r="AC12" s="1">
         <v>2000</v>
       </c>
-      <c r="AB12" s="1">
+      <c r="AD12" s="1">
         <v>2000</v>
       </c>
-      <c r="AC12" s="1">
+      <c r="AE12" s="1">
         <v>2900</v>
       </c>
-      <c r="AD12" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="1" t="s">
+      <c r="AF12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>125</v>
       </c>
@@ -1893,71 +2096,71 @@
       <c r="E13" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="N13" s="1">
-        <v>0</v>
-      </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P13" s="1">
+      <c r="R13" s="1">
         <v>12000</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="S13" s="1">
         <v>210000</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="T13" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="S13" s="1" t="s">
+      <c r="U13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="V13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="U13" s="1">
+      <c r="W13" s="1">
         <v>6</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="X13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W13" s="1" t="s">
+      <c r="Y13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X13" s="1" t="s">
+      <c r="Z13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y13" s="1">
+      <c r="AA13" s="1">
         <v>2</v>
       </c>
-      <c r="Z13" s="1">
+      <c r="AB13" s="1">
         <v>18</v>
       </c>
-      <c r="AA13" s="1">
+      <c r="AC13" s="1">
         <v>2000</v>
       </c>
-      <c r="AB13" s="1">
+      <c r="AD13" s="1">
         <v>2000</v>
       </c>
-      <c r="AC13" s="1">
+      <c r="AE13" s="1">
         <v>2900</v>
       </c>
-      <c r="AD13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE13" s="1" t="s">
+      <c r="AF13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>129</v>
       </c>
@@ -1973,150 +2176,448 @@
       <c r="E14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>2</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="N14" s="1">
-        <v>0</v>
-      </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="P14" s="1">
+      <c r="R14" s="1">
         <v>10400</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="S14" s="1">
         <v>1000</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="T14" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="U14" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="V14" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="U14" s="1" t="s">
+      <c r="W14" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="X14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W14" s="1" t="s">
+      <c r="Y14" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="X14" s="1" t="s">
+      <c r="Z14" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="Y14" s="1">
+      <c r="AA14" s="1">
         <v>2</v>
       </c>
-      <c r="Z14" s="1">
+      <c r="AB14" s="1">
         <v>12</v>
       </c>
-      <c r="AC14" s="1">
+      <c r="AE14" s="1">
         <v>2900</v>
       </c>
-      <c r="AE14" s="1" t="s">
+      <c r="AG14" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R15" s="1">
+        <v>250000</v>
+      </c>
+      <c r="S15" s="1">
+        <v>15000</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>7</v>
+      </c>
+      <c r="AE15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="AG15" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R16" s="1">
+        <v>75000</v>
+      </c>
+      <c r="S16" s="1">
+        <v>8000</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="W16" s="1">
+        <v>4</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>7</v>
+      </c>
+      <c r="AE16" s="1">
+        <v>2000</v>
+      </c>
+      <c r="AG16" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P17" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R17" s="1">
+        <v>100</v>
+      </c>
+      <c r="S17" s="1">
+        <v>100</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="W17" s="1">
+        <v>2</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD17" s="1">
+        <v>200</v>
+      </c>
+      <c r="AE17" s="1">
+        <v>2900</v>
+      </c>
+      <c r="AG17" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A26"/>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A31"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
+      <c r="A33" s="4"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34"/>
+      <c r="A34" s="4"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
+      <c r="A35"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
+      <c r="A36" s="4"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
+      <c r="A37" s="4"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
+      <c r="A38" s="4"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
+      <c r="A40" s="4"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
+      <c r="A41" s="5"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
+      <c r="A42" s="4"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43"/>
+      <c r="A43" s="4"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
+      <c r="A44" s="4"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
+      <c r="A46" s="4"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
+      <c r="A48" s="4"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
+      <c r="A49" s="4"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
+      <c r="A50" s="4"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
+      <c r="A51" s="4"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
+      <c r="A52" s="4"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="3"/>
+      <c r="A53" s="4"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
+      <c r="A54" s="4"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="4"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="4"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="4"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="4"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="4"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="4"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="4"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="4"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="4"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="4"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="4"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="4"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="4"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2125,10 +2626,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2244,7 +2745,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>113</v>
       </c>
       <c r="B11" t="s">
@@ -2284,35 +2785,29 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" t="s">
+        <v>203</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2321,21 +2816,57 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -2348,8 +2879,11 @@
       <c r="D1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -2363,7 +2897,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -2377,7 +2911,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -2391,38 +2925,676 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E22" s="3"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E28" s="3"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5">
+        <v>500</v>
+      </c>
+      <c r="D5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8">
+        <v>240000</v>
+      </c>
+      <c r="D8">
+        <v>240000</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9">
+        <v>200</v>
+      </c>
+      <c r="D9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12">
+        <v>100000</v>
+      </c>
+      <c r="D12">
+        <v>100000</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13" t="s">
+        <v>199</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G3" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" t="s">
+        <v>174</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G5" t="s">
+        <v>183</v>
+      </c>
+      <c r="H5" t="s">
+        <v>174</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" t="s">
+        <v>195</v>
+      </c>
+      <c r="J6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5">
+        <v>4000</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9">
+        <v>1500</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added t1civWasteWaterTank and t1CivWaterTank
</commit_message>
<xml_diff>
--- a/parts/src/main/resources/PARTS.xlsx
+++ b/parts/src/main/resources/PARTS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1880" windowWidth="49640" windowHeight="25040" tabRatio="500"/>
+    <workbookView xWindow="100" yWindow="1880" windowWidth="51100" windowHeight="25040" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PART" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="213">
   <si>
     <t>name</t>
   </si>
@@ -686,6 +686,33 @@
   </si>
   <si>
     <t>CivilianPopulation/Models/Utility/civiedock</t>
+  </si>
+  <si>
+    <t>t1civWasteWaterTank</t>
+  </si>
+  <si>
+    <t>0.0,0, -.6,  0.0, 0, 1, 2</t>
+  </si>
+  <si>
+    <t>Small Waste Water Tank</t>
+  </si>
+  <si>
+    <t>Store the used water from your garden here.</t>
+  </si>
+  <si>
+    <t>wasteWaterContainer , CivilianPopulation/Models/Utility/wasteTank</t>
+  </si>
+  <si>
+    <t>t1CivWaterTank</t>
+  </si>
+  <si>
+    <t>Small Sustenance Tank</t>
+  </si>
+  <si>
+    <t>Store the  food and water for your voyage.</t>
+  </si>
+  <si>
+    <t>wasteWaterContainer , CivilianPopulation/Models/Utility/waterTank</t>
   </si>
 </sst>
 </file>
@@ -757,7 +784,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -767,7 +794,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1049,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG82"/>
+  <dimension ref="A1:AG26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="84" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2229,7 +2255,7 @@
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2451,173 +2477,143 @@
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
+      <c r="A18" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R18" s="1">
+        <v>10400</v>
+      </c>
+      <c r="S18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>12</v>
+      </c>
+      <c r="AE18" s="1">
+        <v>2900</v>
+      </c>
+      <c r="AG18" s="1" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-    </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
+      <c r="A19" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P19" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R19" s="1">
+        <v>10400</v>
+      </c>
+      <c r="S19" s="1">
+        <v>1000</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>12</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>2900</v>
+      </c>
+      <c r="AG19" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A26"/>
       <c r="O26" s="3"/>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A31"/>
-    </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="5"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="4"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="4"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="4"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="4"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="4"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="4"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="4"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="4"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="4"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="4"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="4"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="4"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="4"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="4"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="4"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="4"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="4"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="4"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="4"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="4"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="4"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="4"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="4"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="4"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="4"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="4"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2626,10 +2622,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2801,12 +2797,34 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>188</v>
       </c>
       <c r="B17" t="s">
         <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>209</v>
+      </c>
+      <c r="B19" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -3067,7 +3085,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added more parts to xls file.
</commit_message>
<xml_diff>
--- a/parts/src/main/resources/PARTS.xlsx
+++ b/parts/src/main/resources/PARTS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="100" yWindow="1880" windowWidth="51100" windowHeight="25040" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="7900" windowWidth="51080" windowHeight="20780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="PART" sheetId="1" r:id="rId1"/>
@@ -31,8 +31,31 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="V1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>stack, srfAttach, allowStack, allowSrfAttach, allowCollision</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="340">
   <si>
     <t>name</t>
   </si>
@@ -713,6 +736,409 @@
   </si>
   <si>
     <t>wasteWaterContainer , CivilianPopulation/Models/Utility/waterTank</t>
+  </si>
+  <si>
+    <t>colossalLandingLeg</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>0, 0, 0.0, 1.0, 0.0, 0.0</t>
+  </si>
+  <si>
+    <t>landing</t>
+  </si>
+  <si>
+    <t>Cruiser Landing Gear</t>
+  </si>
+  <si>
+    <t>Netherdyne Aerospace</t>
+  </si>
+  <si>
+    <t>0,1,0,1,0</t>
+  </si>
+  <si>
+    <t>For when you need to land a ship that's simply gigantic, no other gear will do.  Also for keeping bases off the ground.</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Ground/colossalLandingLeg</t>
+  </si>
+  <si>
+    <t>ModuleLandingLeg</t>
+  </si>
+  <si>
+    <t>animationName</t>
+  </si>
+  <si>
+    <t>deployGear</t>
+  </si>
+  <si>
+    <t>wheelColliderName</t>
+  </si>
+  <si>
+    <t>WheelCollider</t>
+  </si>
+  <si>
+    <t>suspensionTransformName</t>
+  </si>
+  <si>
+    <t>pistonMesh</t>
+  </si>
+  <si>
+    <t>suspensionUpperLimit</t>
+  </si>
+  <si>
+    <t>impactTolerance</t>
+  </si>
+  <si>
+    <t>suspensionSpring</t>
+  </si>
+  <si>
+    <t>suspensionDamper</t>
+  </si>
+  <si>
+    <t>colossalLandingLeg2</t>
+  </si>
+  <si>
+    <t>Cruiser Landing Gear Mk2</t>
+  </si>
+  <si>
+    <t>Our second generation of colossal landing legs. For landing even more giant ships and, uh, so on. Sorry; the guy who writes the product descriptions is on vacation.</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Ground/colossalLandingLeg2</t>
+  </si>
+  <si>
+    <t>Deploy</t>
+  </si>
+  <si>
+    <t>Piston</t>
+  </si>
+  <si>
+    <t>orientFootToGround</t>
+  </si>
+  <si>
+    <t>landingFootName</t>
+  </si>
+  <si>
+    <t>FootTransform</t>
+  </si>
+  <si>
+    <t>truss18x18NoCore</t>
+  </si>
+  <si>
+    <t>truss6x18</t>
+  </si>
+  <si>
+    <t>truss6x6Core</t>
+  </si>
+  <si>
+    <t>truss6x6CoreL</t>
+  </si>
+  <si>
+    <t>truss6x6CoreT</t>
+  </si>
+  <si>
+    <t>truss6x6CoreX</t>
+  </si>
+  <si>
+    <t>truss6x6NoCore</t>
+  </si>
+  <si>
+    <t>surfaceAttachHouseSmall</t>
+  </si>
+  <si>
+    <t>6, -9, 0, 0.0, -1.0, 0.0, 3</t>
+  </si>
+  <si>
+    <t>-9,6,0,-1,0,0,3</t>
+  </si>
+  <si>
+    <t>-9, 6, 0.0, -1, 0, 0.0</t>
+  </si>
+  <si>
+    <t>Netherdyne 18m Curved Jumbo Truss</t>
+  </si>
+  <si>
+    <t>Our truck broke down while carrying this.  Cop came up and asked "You buildin a bridge?"  Our driver said "Nope.. rocket."   Look on his face was priceless.</t>
+  </si>
+  <si>
+    <t>1,1,1,1,0</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Structural/truss18x18NoCore</t>
+  </si>
+  <si>
+    <r>
+      <t>Netherdyne</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Monaco"/>
+      </rPr>
+      <t xml:space="preserve"> Aerospace</t>
+    </r>
+  </si>
+  <si>
+    <t>Hester</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Structural/truss6x18</t>
+  </si>
+  <si>
+    <t>0.0, -9, 0.0, 0.0, -1.0, 0.0, 3</t>
+  </si>
+  <si>
+    <t>0.0, 9, 0.0, 0.0, 1.0, 0.0, 3</t>
+  </si>
+  <si>
+    <t>0.0, -9, 0.0, 0.0, -1.0, 0.0</t>
+  </si>
+  <si>
+    <t>Netherdyne Jumbo Truss 18x6</t>
+  </si>
+  <si>
+    <t>We shut down at least three major interstates with the convoy that carried this here.</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Structural/truss6x6Core</t>
+  </si>
+  <si>
+    <t>1, 1, 1</t>
+  </si>
+  <si>
+    <t>0.0, -3, 0.0, 0.0, -1.0, 0.0, 3</t>
+  </si>
+  <si>
+    <t>0.0, 3, 0.0, 0.0, 1.0, 0.0, 3</t>
+  </si>
+  <si>
+    <t>3,0,0,1,0,0,3</t>
+  </si>
+  <si>
+    <t>-3,0,0,-1,0,0,3</t>
+  </si>
+  <si>
+    <t>0,0,-3,0,0,-1,3</t>
+  </si>
+  <si>
+    <t>0,0,3,0,0,1,3</t>
+  </si>
+  <si>
+    <t>0.0, -3, 0.0, 0.0, -1.0, 0.0</t>
+  </si>
+  <si>
+    <t>Netherdyne Jumbo Truss 6x6 (with core)</t>
+  </si>
+  <si>
+    <t>Tired of customer complaints about having to cut through massive pieces of girdering in order to create passageways, Netherdyne decided to build them right in. This enormous cube-ish girder segment comes complete with a hull section suitable for kerbonauts and civilians to pass through. Please do not loiter in the girder.</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Structural/truss6x6CoreL</t>
+  </si>
+  <si>
+    <t>Netherdyne Jumbo Truss 6x6 Bend (with Core)</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Structural/truss6x6CoreT</t>
+  </si>
+  <si>
+    <t>Netherdyne Jumbo Truss 6x6 T Junction (with Core)</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Structural/truss6x6CoreX</t>
+  </si>
+  <si>
+    <t>Netherdyne Jumbo Truss 6x6 Junction (with Core)</t>
+  </si>
+  <si>
+    <t>Hester, Cosmic Farmer, Rabidninjawombat</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Structural/truss6x6NoCore</t>
+  </si>
+  <si>
+    <t>Netherdyne Jumbo Truss 6x6</t>
+  </si>
+  <si>
+    <t>You know your space ship is huge when a part of it gets hauled into the VAB with Wide Load signs on it. Made from ultra-high tensile alloys, this truss piece is designed to withstand the crushing force of super-heavy structures.</t>
+  </si>
+  <si>
+    <t>InsituKerbalRecruiterTest</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Utility/CiviHousing_Size2_01</t>
+  </si>
+  <si>
+    <t>smallApartmentInternal</t>
+  </si>
+  <si>
+    <t>Hester, Cosmic Farmer</t>
+  </si>
+  <si>
+    <t>0.0, 2, 0.0, 0.0, 1.0, 0.0, 3</t>
+  </si>
+  <si>
+    <t>0.0, -2, 0.0, 0.0, -1.0, 0.0, 3</t>
+  </si>
+  <si>
+    <t>0.0, -2, 0, 0.0, -1.0, 0, 3</t>
+  </si>
+  <si>
+    <t>Civilian Large House mk2</t>
+  </si>
+  <si>
+    <t>Intended for the house owner on the up, or the station developer on a budget, this cozy habitation pod has long-term living space for up to 8 kerbals.</t>
+  </si>
+  <si>
+    <t>0.000000185</t>
+  </si>
+  <si>
+    <t>CivilianSpawnGrowth</t>
+  </si>
+  <si>
+    <t>ModuleScienceContainer</t>
+  </si>
+  <si>
+    <t>reviewActionName</t>
+  </si>
+  <si>
+    <t>storeActionName</t>
+  </si>
+  <si>
+    <t>collectActionName</t>
+  </si>
+  <si>
+    <t>evaOnlyStorage</t>
+  </si>
+  <si>
+    <t>storageRange</t>
+  </si>
+  <si>
+    <t>allowRepeatedSubjects</t>
+  </si>
+  <si>
+    <t>Take Data</t>
+  </si>
+  <si>
+    <t>Store Experiments</t>
+  </si>
+  <si>
+    <t>Review Data</t>
+  </si>
+  <si>
+    <t>blank_1 , Squad/Parts/Utility/dockingPortSr/model000
+blank_1_NRM , Squad/Parts/Utility/dockingPortSr/model001</t>
+  </si>
+  <si>
+    <t>t1CivilizationGenerationShipQuartersMedium</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Utility/CiviHousing_Size3_01</t>
+  </si>
+  <si>
+    <t>blank_1 , Squad/Parts/Command/mk1LanderCan/ksp_s_landerCan_diff
+blank_1_NRM , Squad/Parts/Command/mk1LanderCan/ksp_s_landerCan_normal</t>
+  </si>
+  <si>
+    <t>mediumQuartersInternal</t>
+  </si>
+  <si>
+    <t>0.0, 3.5, 0.0, 0.0, 1.0, 0.0, 3</t>
+  </si>
+  <si>
+    <t>0.0, -3.5, 0.0, 0.0, -1.0, 0.0, 3</t>
+  </si>
+  <si>
+    <t>advExploration</t>
+  </si>
+  <si>
+    <t>Civilian Small Apartment Complex</t>
+  </si>
+  <si>
+    <t>25 willing victims...err guests travel in style in this retro quarters.</t>
+  </si>
+  <si>
+    <t>Hester, Cosmic Farmer, RabidNinjaWombat</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Utility/CiviHousing_Size4</t>
+  </si>
+  <si>
+    <t>t1CivilizationGenerationShipQuartersLarge</t>
+  </si>
+  <si>
+    <t>0.0, 6.75, 0.0, 0.0, 1.0, 0.0, 3</t>
+  </si>
+  <si>
+    <t>0.0, -6.75, 0.0, 0.0, -1.0, 0.0, 4</t>
+  </si>
+  <si>
+    <t>0.0,-6.75, 0,  0.0, -1, 0, 3</t>
+  </si>
+  <si>
+    <t>Civilian Large Apartment Complex</t>
+  </si>
+  <si>
+    <t>Come and stay in our luxurious apartments among the stars.  Whether in orbit or on the surface, our apartments offer 5-star accommodation, with communal lounge, bar and gymnasium. Our extravagant viewing deck provides a panorama you can't get anywhere else. This building houses 60 civilians, and has enough space to accommodate 8 crew members.</t>
+  </si>
+  <si>
+    <t>FlagDecal</t>
+  </si>
+  <si>
+    <t>textureQuadName</t>
+  </si>
+  <si>
+    <t>Flag_1</t>
+  </si>
+  <si>
+    <t>Flag_2</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Utility/surfaceAttachHouseSmall</t>
+  </si>
+  <si>
+    <t>0.0, 0.7, 0.0, 0.0, 1.0, 0.0, 2</t>
+  </si>
+  <si>
+    <t>0.0, -0.7, 0.0, 0.0, -1.0, 0.0, 2</t>
+  </si>
+  <si>
+    <t>0.0, -0.7, 0, 0.0, -1, 0, 2</t>
+  </si>
+  <si>
+    <t>Civilian Small House</t>
+  </si>
+  <si>
+    <t>Netherdyne KR department</t>
+  </si>
+  <si>
+    <t>Attach this small house to any ship or base.  Also goes great in a biodome.</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>Review Stored Data</t>
+  </si>
+  <si>
+    <r>
+      <t>hester</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Monaco"/>
+      </rPr>
+      <t>,Cosmic_Farmer,RabidNinjaWombat</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -755,9 +1181,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF2600"/>
-      <name val="Monaco"/>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -784,7 +1211,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -792,7 +1219,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
@@ -1074,16 +1500,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG32"/>
   <sheetViews>
-    <sheetView zoomScale="84" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
@@ -1534,7 +1960,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>62</v>
       </c>
@@ -2612,219 +3038,1440 @@
         <v>211</v>
       </c>
     </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="R20" s="1">
+        <v>2200</v>
+      </c>
+      <c r="S20" s="1">
+        <v>2500</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="W20" s="1">
+        <v>4</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>80</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>800</v>
+      </c>
+      <c r="AD20" s="1">
+        <v>8000</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>2900</v>
+      </c>
+      <c r="AF20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="R21" s="1">
+        <v>2200</v>
+      </c>
+      <c r="S21" s="1">
+        <v>2500</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="W21" s="1">
+        <v>3</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>80</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>800</v>
+      </c>
+      <c r="AD21" s="1">
+        <v>8000</v>
+      </c>
+      <c r="AE21" s="1">
+        <v>2900</v>
+      </c>
+      <c r="AF21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R22" s="1">
+        <v>7800</v>
+      </c>
+      <c r="S22" s="1">
+        <v>2000</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="W22" s="1">
+        <v>18</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>80</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>200</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>3000</v>
+      </c>
+      <c r="AG22" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R23" s="1">
+        <v>7800</v>
+      </c>
+      <c r="S23" s="1">
+        <v>2000</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="W23" s="1">
+        <v>12</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>80</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>200</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>3000</v>
+      </c>
+      <c r="AG23" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R24" s="1">
+        <v>7800</v>
+      </c>
+      <c r="S24" s="1">
+        <v>2000</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="W24" s="1">
+        <v>7</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>80</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD24" s="1">
+        <v>200</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>3000</v>
+      </c>
+      <c r="AG24" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R25" s="1">
+        <v>7800</v>
+      </c>
+      <c r="S25" s="1">
+        <v>2000</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="W25" s="1">
+        <v>9</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>80</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>200</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>3000</v>
+      </c>
+      <c r="AG25" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="O26" s="3"/>
+      <c r="A26" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R26" s="1">
+        <v>7800</v>
+      </c>
+      <c r="S26" s="1">
+        <v>2000</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="W26" s="1">
+        <v>9</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>80</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD26" s="1">
+        <v>200</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>3000</v>
+      </c>
+      <c r="AG26" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R27" s="1">
+        <v>7800</v>
+      </c>
+      <c r="S27" s="1">
+        <v>2000</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="W27" s="1">
+        <v>9</v>
+      </c>
+      <c r="X27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>80</v>
+      </c>
+      <c r="AC27" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD27" s="1">
+        <v>200</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>3000</v>
+      </c>
+      <c r="AG27" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R28" s="1">
+        <v>7800</v>
+      </c>
+      <c r="S28" s="1">
+        <v>2000</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="W28" s="1">
+        <v>4</v>
+      </c>
+      <c r="X28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>80</v>
+      </c>
+      <c r="AC28" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD28" s="1">
+        <v>200</v>
+      </c>
+      <c r="AE28" s="1">
+        <v>3000</v>
+      </c>
+      <c r="AG28" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="P29" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R29" s="1">
+        <v>10400</v>
+      </c>
+      <c r="S29" s="1">
+        <v>13500</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="W29" s="1">
+        <v>2</v>
+      </c>
+      <c r="X29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA29" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB29" s="1">
+        <v>12</v>
+      </c>
+      <c r="AC29" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD29" s="1">
+        <v>200</v>
+      </c>
+      <c r="AE29" s="1">
+        <v>2900</v>
+      </c>
+      <c r="AG29" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="P30" s="1">
+        <v>25</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="R30" s="1">
+        <v>10400</v>
+      </c>
+      <c r="S30" s="1">
+        <v>80000</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="U30" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="W30" s="1">
+        <v>5</v>
+      </c>
+      <c r="X30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA30" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB30" s="1">
+        <v>14</v>
+      </c>
+      <c r="AC30" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD30" s="1">
+        <v>200</v>
+      </c>
+      <c r="AE30" s="1">
+        <v>2900</v>
+      </c>
+      <c r="AG30" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="P31" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R31" s="1">
+        <v>10400</v>
+      </c>
+      <c r="S31" s="1">
+        <v>160000</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="W31" s="1">
+        <v>15</v>
+      </c>
+      <c r="X31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA31" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB31" s="1">
+        <v>16</v>
+      </c>
+      <c r="AC31" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD31" s="1">
+        <v>200</v>
+      </c>
+      <c r="AE31" s="1">
+        <v>2900</v>
+      </c>
+      <c r="AG31" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="P32" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R32" s="1">
+        <v>10400</v>
+      </c>
+      <c r="S32" s="1">
+        <v>13500</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="U32" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="W32" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="X32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA32" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB32" s="1">
+        <v>12</v>
+      </c>
+      <c r="AC32" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD32" s="1">
+        <v>200</v>
+      </c>
+      <c r="AE32" s="1">
+        <v>2900</v>
+      </c>
+      <c r="AG32" s="1" t="s">
+        <v>335</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -2834,16 +4481,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -2860,6 +4507,38 @@
       </c>
       <c r="B2" t="s">
         <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>319</v>
+      </c>
+      <c r="B5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B6" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2869,15 +4548,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
@@ -3062,7 +4741,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>188</v>
       </c>
       <c r="B13" t="s">
@@ -3072,6 +4751,62 @@
         <v>0</v>
       </c>
       <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>286</v>
+      </c>
+      <c r="B14" t="s">
+        <v>199</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>308</v>
+      </c>
+      <c r="B15" t="s">
+        <v>199</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>319</v>
+      </c>
+      <c r="B16" t="s">
+        <v>199</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>249</v>
+      </c>
+      <c r="B17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
         <v>2</v>
       </c>
     </row>
@@ -3082,15 +4817,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
@@ -3100,9 +4835,25 @@
     <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -3133,8 +4884,56 @@
       <c r="J1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>223</v>
+      </c>
+      <c r="L1" t="s">
+        <v>225</v>
+      </c>
+      <c r="M1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N1" t="s">
+        <v>229</v>
+      </c>
+      <c r="O1" t="s">
+        <v>230</v>
+      </c>
+      <c r="P1" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>232</v>
+      </c>
+      <c r="R1" t="s">
+        <v>239</v>
+      </c>
+      <c r="S1" t="s">
+        <v>240</v>
+      </c>
+      <c r="T1" t="s">
+        <v>298</v>
+      </c>
+      <c r="U1" t="s">
+        <v>299</v>
+      </c>
+      <c r="V1" t="s">
+        <v>300</v>
+      </c>
+      <c r="W1" t="s">
+        <v>301</v>
+      </c>
+      <c r="X1" t="s">
+        <v>302</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>303</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>142</v>
       </c>
@@ -3151,7 +4950,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -3171,8 +4970,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>178</v>
       </c>
       <c r="B4" t="s">
@@ -3188,8 +4987,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>178</v>
       </c>
       <c r="B5" t="s">
@@ -3208,8 +5007,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>188</v>
       </c>
       <c r="B6" t="s">
@@ -3219,136 +5018,241 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>188</v>
       </c>
       <c r="B7" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="4"/>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8" t="s">
+        <v>222</v>
+      </c>
+      <c r="K8" t="s">
+        <v>224</v>
+      </c>
+      <c r="L8" t="s">
+        <v>226</v>
+      </c>
+      <c r="M8" t="s">
+        <v>228</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>20000</v>
+      </c>
+      <c r="P8">
+        <v>100</v>
+      </c>
+      <c r="Q8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>233</v>
+      </c>
+      <c r="B9" t="s">
+        <v>222</v>
+      </c>
+      <c r="K9" t="s">
+        <v>237</v>
+      </c>
+      <c r="L9" t="s">
+        <v>226</v>
+      </c>
+      <c r="M9" t="s">
+        <v>238</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>20000</v>
+      </c>
+      <c r="P9">
+        <v>100</v>
+      </c>
+      <c r="Q9">
+        <v>55</v>
+      </c>
+      <c r="R9" t="b">
+        <v>1</v>
+      </c>
+      <c r="S9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>286</v>
+      </c>
+      <c r="B10" t="s">
+        <v>296</v>
+      </c>
+      <c r="J10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>286</v>
+      </c>
+      <c r="B11" t="s">
+        <v>297</v>
+      </c>
+      <c r="T11" t="s">
+        <v>306</v>
+      </c>
+      <c r="U11" t="s">
+        <v>305</v>
+      </c>
+      <c r="V11" t="s">
+        <v>304</v>
+      </c>
+      <c r="W11" t="b">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>2</v>
+      </c>
+      <c r="Y11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>308</v>
+      </c>
+      <c r="B12" t="s">
+        <v>296</v>
+      </c>
+      <c r="J12" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>308</v>
+      </c>
+      <c r="B13" t="s">
+        <v>297</v>
+      </c>
+      <c r="T13" t="s">
+        <v>306</v>
+      </c>
+      <c r="U13" t="s">
+        <v>305</v>
+      </c>
+      <c r="V13" t="s">
+        <v>304</v>
+      </c>
+      <c r="W13" t="b">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <v>2</v>
+      </c>
+      <c r="Y13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>319</v>
+      </c>
+      <c r="B14" t="s">
+        <v>296</v>
+      </c>
+      <c r="J14" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>319</v>
+      </c>
+      <c r="B15" t="s">
+        <v>297</v>
+      </c>
+      <c r="T15" t="s">
+        <v>306</v>
+      </c>
+      <c r="U15" t="s">
+        <v>305</v>
+      </c>
+      <c r="V15" t="s">
+        <v>304</v>
+      </c>
+      <c r="W15" t="b">
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <v>2</v>
+      </c>
+      <c r="Y15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>319</v>
+      </c>
+      <c r="B16" t="s">
+        <v>325</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>319</v>
+      </c>
+      <c r="B17" t="s">
+        <v>325</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>249</v>
+      </c>
+      <c r="B18" t="s">
+        <v>296</v>
+      </c>
+      <c r="J18" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>249</v>
+      </c>
+      <c r="B19" t="s">
+        <v>297</v>
+      </c>
+      <c r="T19" t="s">
+        <v>338</v>
+      </c>
+      <c r="U19" t="s">
+        <v>305</v>
+      </c>
+      <c r="W19" t="b">
+        <v>1</v>
+      </c>
+      <c r="X19" t="s">
+        <v>337</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3546,73 +5450,73 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
+      <c r="A10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
+      <c r="A11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
+      <c r="A12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
+      <c r="A13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
+      <c r="A15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
+      <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
+      <c r="A17" s="3"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
+      <c r="A18" s="3"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
+      <c r="A19" s="3"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
+      <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
+      <c r="A21" s="3"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
+      <c r="A22" s="3"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
+      <c r="A23" s="3"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
+      <c r="A24" s="3"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
+      <c r="A25" s="3"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
+      <c r="A26" s="3"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
+      <c r="A27" s="3"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
+      <c r="A28" s="3"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
+      <c r="A29" s="3"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
+      <c r="A30" s="3"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
+      <c r="A31" s="3"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
+      <c r="A32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added t1civGardenBiosphereMedium & t1civGardenBiosphere
</commit_message>
<xml_diff>
--- a/parts/src/main/resources/PARTS.xlsx
+++ b/parts/src/main/resources/PARTS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7900" windowWidth="51080" windowHeight="20780" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="11540" windowWidth="51080" windowHeight="17140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PART" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="386">
   <si>
     <t>name</t>
   </si>
@@ -1307,12 +1307,48 @@
   <si>
     <t>allowManualControl</t>
   </si>
+  <si>
+    <t>t1civGardenBiosphereMedium</t>
+  </si>
+  <si>
+    <t>t1civGardenBiosphere</t>
+  </si>
+  <si>
+    <t>0.0, 4.25, 0.0, 0.0, 1.0, 0.0, 4</t>
+  </si>
+  <si>
+    <t>0.0, -4.25, 0.0, 0.0, -1.0, 0.0, 4</t>
+  </si>
+  <si>
+    <t>Small Hydroponic Garden Biosphere</t>
+  </si>
+  <si>
+    <t>Combining new advances in Direct-to-Root (TM) hydroponics technology with traditional agriculture and the ancient art of origami, Netherdyne presents the Small Garden Biosphere. A step up from our smaller hydroponics range, this computer-controlled unit allows forming a complete biosphere for several families of kerbals. By folding the garden in on itself, we've compacted it into a handy sphere, suitable for integration into any large space station. Supports up to 25 civilians.</t>
+  </si>
+  <si>
+    <t>0.0, 10.17, 0.0, 0.0, 1.0, 0.0, 5</t>
+  </si>
+  <si>
+    <t>0.0, -10.14, 0.0, 0.0, -1.0, 0.0, 5</t>
+  </si>
+  <si>
+    <t>Hydroponic Garden Biosphere</t>
+  </si>
+  <si>
+    <t>The cornerstone of your generation ship or space station the Hydroponic Garden Biosphere provides enough food for 50 civilians.</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Utility/Hydroponics_Medium_01</t>
+  </si>
+  <si>
+    <t>CivilianPopulation/Models/Utility/Hydroponics_Large_01</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1358,6 +1394,11 @@
       <color rgb="FFFF2600"/>
       <name val="Monaco"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3933FF"/>
+      <name val="Monaco"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1383,7 +1424,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1394,6 +1435,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1675,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG34"/>
+  <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView zoomScale="84" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="P2" zoomScale="84" workbookViewId="0">
+      <selection activeCell="AB37" sqref="AB37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4469,6 +4511,168 @@
         <v>368</v>
       </c>
     </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="P35" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="R35" s="1">
+        <v>10400</v>
+      </c>
+      <c r="S35" s="5">
+        <v>75000</v>
+      </c>
+      <c r="T35" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="U35" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="V35" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="W35" s="5">
+        <v>10</v>
+      </c>
+      <c r="X35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA35" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB35" s="5">
+        <v>10</v>
+      </c>
+      <c r="AC35" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD35" s="1">
+        <v>200</v>
+      </c>
+      <c r="AE35" s="1">
+        <v>2900</v>
+      </c>
+      <c r="AG35" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="P36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="R36" s="1">
+        <v>10400</v>
+      </c>
+      <c r="S36" s="5">
+        <v>180000</v>
+      </c>
+      <c r="T36" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="U36" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="V36" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="W36" s="5">
+        <v>20</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA36" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB36" s="1">
+        <v>14</v>
+      </c>
+      <c r="AC36" s="1">
+        <v>200</v>
+      </c>
+      <c r="AD36" s="1">
+        <v>200</v>
+      </c>
+      <c r="AE36" s="1">
+        <v>2900</v>
+      </c>
+      <c r="AG36" s="5" t="s">
+        <v>383</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4477,10 +4681,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4836,6 +5040,28 @@
         <v>266</v>
       </c>
       <c r="D34" s="5" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>366</v>
       </c>
     </row>
@@ -4921,10 +5147,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5267,6 +5493,34 @@
         <v>50</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24">
+        <v>200</v>
+      </c>
+      <c r="D24">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="B25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25">
+        <v>400</v>
+      </c>
+      <c r="D25">
+        <v>400</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5276,8 +5530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Kerbalims config for t1civSmallGardenModule
</commit_message>
<xml_diff>
--- a/parts/src/main/resources/PARTS.xlsx
+++ b/parts/src/main/resources/PARTS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="18740" windowWidth="51080" windowHeight="9940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="18740" windowWidth="51080" windowHeight="9940" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PART" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="436">
   <si>
     <t>name</t>
   </si>
@@ -1855,9 +1855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+    <sheetView zoomScale="84" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T38" sqref="T37:T38"/>
+      <selection pane="bottomLeft" activeCell="AA34" sqref="AA34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5440,10 +5440,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5770,48 +5770,6 @@
       </c>
       <c r="D22">
         <v>1000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>362</v>
-      </c>
-      <c r="B23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C23">
-        <v>50</v>
-      </c>
-      <c r="D23">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>374</v>
-      </c>
-      <c r="B24" t="s">
-        <v>109</v>
-      </c>
-      <c r="C24">
-        <v>200</v>
-      </c>
-      <c r="D24">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>375</v>
-      </c>
-      <c r="B25" t="s">
-        <v>109</v>
-      </c>
-      <c r="C25">
-        <v>400</v>
-      </c>
-      <c r="D25">
-        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The service now knows if a vessel has a civilian dock.
</commit_message>
<xml_diff>
--- a/parts/src/main/resources/PARTS.xlsx
+++ b/parts/src/main/resources/PARTS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8900" windowWidth="47400" windowHeight="19580" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="8900" windowWidth="47400" windowHeight="19580" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="PART" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="A13" authorId="0">
+    <comment ref="A14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="437">
   <si>
     <t>name</t>
   </si>
@@ -1548,6 +1548,9 @@
   </si>
   <si>
     <t>CivilianPopulation/Models/Utility/laserDrill</t>
+  </si>
+  <si>
+    <t>CivilianPopulationDockModule</t>
   </si>
 </sst>
 </file>
@@ -1913,7 +1916,7 @@
   <sheetViews>
     <sheetView zoomScale="84" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20:C21"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5016,8 +5019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5498,8 +5501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5835,11 +5838,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ29"/>
+  <dimension ref="A1:AQ30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6054,33 +6057,18 @@
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>286</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>297</v>
-      </c>
-      <c r="T4" t="s">
-        <v>306</v>
-      </c>
-      <c r="U4" t="s">
-        <v>305</v>
-      </c>
-      <c r="V4" t="s">
-        <v>304</v>
-      </c>
-      <c r="W4" t="b">
-        <v>1</v>
-      </c>
-      <c r="X4">
-        <v>2</v>
-      </c>
-      <c r="Y4" t="b">
-        <v>1</v>
+        <v>436</v>
+      </c>
+      <c r="J4" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>308</v>
+        <v>286</v>
       </c>
       <c r="B5" t="s">
         <v>297</v>
@@ -6106,7 +6094,7 @@
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="B6" t="s">
         <v>297</v>
@@ -6135,10 +6123,25 @@
         <v>319</v>
       </c>
       <c r="B7" t="s">
-        <v>325</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>327</v>
+        <v>297</v>
+      </c>
+      <c r="T7" t="s">
+        <v>306</v>
+      </c>
+      <c r="U7" t="s">
+        <v>305</v>
+      </c>
+      <c r="V7" t="s">
+        <v>304</v>
+      </c>
+      <c r="W7" t="b">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>2</v>
+      </c>
+      <c r="Y7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.2">
@@ -6149,38 +6152,38 @@
         <v>325</v>
       </c>
       <c r="Z8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>249</v>
+        <v>319</v>
       </c>
       <c r="B9" t="s">
-        <v>297</v>
-      </c>
-      <c r="T9" t="s">
-        <v>338</v>
-      </c>
-      <c r="U9" t="s">
-        <v>305</v>
-      </c>
-      <c r="W9" t="b">
-        <v>1</v>
-      </c>
-      <c r="X9" t="s">
-        <v>337</v>
+        <v>325</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>340</v>
+        <v>249</v>
       </c>
       <c r="B10" t="s">
-        <v>347</v>
-      </c>
-      <c r="AA10">
-        <v>0</v>
+        <v>297</v>
+      </c>
+      <c r="T10" t="s">
+        <v>338</v>
+      </c>
+      <c r="U10" t="s">
+        <v>305</v>
+      </c>
+      <c r="W10" t="b">
+        <v>1</v>
+      </c>
+      <c r="X10" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.2">
@@ -6188,25 +6191,10 @@
         <v>340</v>
       </c>
       <c r="B11" t="s">
-        <v>297</v>
-      </c>
-      <c r="T11" t="s">
-        <v>306</v>
-      </c>
-      <c r="U11" t="s">
-        <v>305</v>
-      </c>
-      <c r="V11" t="s">
-        <v>304</v>
-      </c>
-      <c r="W11" t="b">
-        <v>1</v>
-      </c>
-      <c r="X11">
-        <v>2</v>
-      </c>
-      <c r="Y11" t="b">
-        <v>1</v>
+        <v>347</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.2">
@@ -6214,77 +6202,77 @@
         <v>340</v>
       </c>
       <c r="B12" t="s">
-        <v>349</v>
-      </c>
-      <c r="AB12">
+        <v>297</v>
+      </c>
+      <c r="T12" t="s">
+        <v>306</v>
+      </c>
+      <c r="U12" t="s">
+        <v>305</v>
+      </c>
+      <c r="V12" t="s">
+        <v>304</v>
+      </c>
+      <c r="W12" t="b">
         <v>1</v>
       </c>
-      <c r="AC12">
-        <v>500</v>
-      </c>
-      <c r="AD12">
+      <c r="X12">
+        <v>2</v>
+      </c>
+      <c r="Y12" t="b">
         <v>1</v>
-      </c>
-      <c r="AE12" t="b">
-        <v>1</v>
-      </c>
-      <c r="AF12" t="b">
-        <v>1</v>
-      </c>
-      <c r="AG12">
-        <v>5</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>137</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>355</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>362</v>
+        <v>340</v>
       </c>
       <c r="B13" t="s">
-        <v>369</v>
-      </c>
-      <c r="K13" t="s">
-        <v>370</v>
-      </c>
-      <c r="AK13" t="s">
-        <v>372</v>
-      </c>
-      <c r="AL13" t="b">
-        <v>0</v>
+        <v>349</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+      <c r="AC13">
+        <v>500</v>
+      </c>
+      <c r="AD13">
+        <v>1</v>
+      </c>
+      <c r="AE13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG13">
+        <v>5</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>355</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
       <c r="B14" t="s">
-        <v>394</v>
-      </c>
-      <c r="C14" t="s">
-        <v>397</v>
-      </c>
-      <c r="D14" t="s">
-        <v>398</v>
-      </c>
-      <c r="E14" t="s">
-        <v>399</v>
-      </c>
-      <c r="AM14">
-        <v>0</v>
-      </c>
-      <c r="AN14">
-        <v>24</v>
-      </c>
-      <c r="AO14" t="s">
-        <v>138</v>
+        <v>369</v>
+      </c>
+      <c r="K14" t="s">
+        <v>370</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>372</v>
+      </c>
+      <c r="AL14" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.2">
@@ -6295,13 +6283,13 @@
         <v>394</v>
       </c>
       <c r="C15" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D15" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="E15" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="AM15">
         <v>0</v>
@@ -6310,7 +6298,7 @@
         <v>24</v>
       </c>
       <c r="AO15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.2">
@@ -6321,13 +6309,13 @@
         <v>394</v>
       </c>
       <c r="C16" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D16" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="E16" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="AM16">
         <v>0</v>
@@ -6336,7 +6324,7 @@
         <v>24</v>
       </c>
       <c r="AO16" t="s">
-        <v>420</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.2">
@@ -6347,13 +6335,13 @@
         <v>394</v>
       </c>
       <c r="C17" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D17" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E17" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="AM17">
         <v>0</v>
@@ -6362,10 +6350,7 @@
         <v>24</v>
       </c>
       <c r="AO17" t="s">
-        <v>421</v>
-      </c>
-      <c r="AP17" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.2">
@@ -6376,13 +6361,13 @@
         <v>394</v>
       </c>
       <c r="C18" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D18" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E18" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="AM18">
         <v>0</v>
@@ -6391,13 +6376,10 @@
         <v>24</v>
       </c>
       <c r="AO18" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="AP18" t="s">
         <v>426</v>
-      </c>
-      <c r="AQ18" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.2">
@@ -6408,13 +6390,13 @@
         <v>394</v>
       </c>
       <c r="C19" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D19" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="E19" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="AM19">
         <v>0</v>
@@ -6423,7 +6405,13 @@
         <v>24</v>
       </c>
       <c r="AO19" t="s">
-        <v>423</v>
+        <v>422</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>426</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.2">
@@ -6434,13 +6422,13 @@
         <v>394</v>
       </c>
       <c r="C20" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D20" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E20" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AM20">
         <v>0</v>
@@ -6449,13 +6437,7 @@
         <v>24</v>
       </c>
       <c r="AO20" t="s">
-        <v>424</v>
-      </c>
-      <c r="AP20" t="s">
-        <v>426</v>
-      </c>
-      <c r="AQ20" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.2">
@@ -6463,42 +6445,48 @@
         <v>386</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
-      </c>
-      <c r="F21" t="s">
-        <v>400</v>
-      </c>
-      <c r="G21" t="s">
-        <v>184</v>
-      </c>
-      <c r="H21" t="s">
-        <v>401</v>
+        <v>394</v>
+      </c>
+      <c r="C21" t="s">
+        <v>417</v>
+      </c>
+      <c r="D21" t="s">
+        <v>418</v>
+      </c>
+      <c r="E21" t="s">
+        <v>419</v>
+      </c>
+      <c r="AM21">
+        <v>0</v>
+      </c>
+      <c r="AN21">
+        <v>24</v>
+      </c>
+      <c r="AO21" t="s">
+        <v>424</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>426</v>
+      </c>
+      <c r="AQ21" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B22" t="s">
-        <v>394</v>
-      </c>
-      <c r="C22" t="s">
-        <v>397</v>
-      </c>
-      <c r="D22" t="s">
-        <v>398</v>
-      </c>
-      <c r="E22" t="s">
-        <v>399</v>
-      </c>
-      <c r="AM22">
-        <v>0</v>
-      </c>
-      <c r="AN22">
-        <v>4</v>
-      </c>
-      <c r="AO22" t="s">
-        <v>138</v>
+        <v>171</v>
+      </c>
+      <c r="F22" t="s">
+        <v>400</v>
+      </c>
+      <c r="G22" t="s">
+        <v>184</v>
+      </c>
+      <c r="H22" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.2">
@@ -6509,13 +6497,13 @@
         <v>394</v>
       </c>
       <c r="C23" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D23" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="E23" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="AM23">
         <v>0</v>
@@ -6524,7 +6512,7 @@
         <v>4</v>
       </c>
       <c r="AO23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.2">
@@ -6535,13 +6523,13 @@
         <v>394</v>
       </c>
       <c r="C24" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D24" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="E24" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="AM24">
         <v>0</v>
@@ -6550,7 +6538,7 @@
         <v>4</v>
       </c>
       <c r="AO24" t="s">
-        <v>420</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.2">
@@ -6561,13 +6549,13 @@
         <v>394</v>
       </c>
       <c r="C25" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D25" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E25" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="AM25">
         <v>0</v>
@@ -6576,10 +6564,7 @@
         <v>4</v>
       </c>
       <c r="AO25" t="s">
-        <v>421</v>
-      </c>
-      <c r="AP25" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.2">
@@ -6590,13 +6575,13 @@
         <v>394</v>
       </c>
       <c r="C26" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D26" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E26" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="AM26">
         <v>0</v>
@@ -6605,13 +6590,10 @@
         <v>4</v>
       </c>
       <c r="AO26" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="AP26" t="s">
         <v>426</v>
-      </c>
-      <c r="AQ26" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.2">
@@ -6622,13 +6604,13 @@
         <v>394</v>
       </c>
       <c r="C27" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D27" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="E27" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="AM27">
         <v>0</v>
@@ -6637,7 +6619,13 @@
         <v>4</v>
       </c>
       <c r="AO27" t="s">
-        <v>423</v>
+        <v>422</v>
+      </c>
+      <c r="AP27" t="s">
+        <v>426</v>
+      </c>
+      <c r="AQ27" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.2">
@@ -6648,13 +6636,13 @@
         <v>394</v>
       </c>
       <c r="C28" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D28" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E28" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AM28">
         <v>0</v>
@@ -6663,13 +6651,7 @@
         <v>4</v>
       </c>
       <c r="AO28" t="s">
-        <v>424</v>
-      </c>
-      <c r="AP28" t="s">
-        <v>426</v>
-      </c>
-      <c r="AQ28" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.2">
@@ -6677,15 +6659,47 @@
         <v>387</v>
       </c>
       <c r="B29" t="s">
+        <v>394</v>
+      </c>
+      <c r="C29" t="s">
+        <v>417</v>
+      </c>
+      <c r="D29" t="s">
+        <v>418</v>
+      </c>
+      <c r="E29" t="s">
+        <v>419</v>
+      </c>
+      <c r="AM29">
+        <v>0</v>
+      </c>
+      <c r="AN29">
+        <v>4</v>
+      </c>
+      <c r="AO29" t="s">
+        <v>424</v>
+      </c>
+      <c r="AP29" t="s">
+        <v>426</v>
+      </c>
+      <c r="AQ29" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>387</v>
+      </c>
+      <c r="B30" t="s">
         <v>171</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>237</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G30" t="s">
         <v>401</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H30" t="s">
         <v>401</v>
       </c>
     </row>
@@ -6700,10 +6714,14 @@
   <dimension ref="A1:AQ40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AQ40"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>